<commit_message>
updated to mission 2032
</commit_message>
<xml_diff>
--- a/Specialist_Mission_BoBs.xlsx
+++ b/Specialist_Mission_BoBs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2220" yWindow="0" windowWidth="25040" windowHeight="16500" tabRatio="500"/>
+    <workbookView xWindow="1300" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Specialist_Mission_BoBs.csv" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="597" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="615" uniqueCount="134">
   <si>
     <t>Veil</t>
   </si>
@@ -30,9 +30,6 @@
     <t>ex0</t>
   </si>
   <si>
-    <t>AYBAB</t>
-  </si>
-  <si>
     <t>Shogun</t>
   </si>
   <si>
@@ -415,6 +412,15 @@
   </si>
   <si>
     <t>Ciacona</t>
+  </si>
+  <si>
+    <t>AYBABTU</t>
+  </si>
+  <si>
+    <t>Xavis</t>
+  </si>
+  <si>
+    <t>Kissing Emoji</t>
   </si>
 </sst>
 </file>
@@ -463,17 +469,29 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="9">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -803,23 +821,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C298"/>
+  <dimension ref="A1:C307"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A252" workbookViewId="0">
-      <selection activeCell="C261" sqref="C261"/>
+    <sheetView tabSelected="1" topLeftCell="A281" workbookViewId="0">
+      <selection activeCell="A308" sqref="A308"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B1" t="s">
         <v>127</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>128</v>
-      </c>
-      <c r="C1" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -842,7 +860,7 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>3</v>
+        <v>131</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -851,7 +869,7 @@
         <v>272</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C4" t="s">
         <v>1</v>
@@ -863,10 +881,10 @@
         <v>273</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -875,10 +893,10 @@
         <v>274</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -887,10 +905,10 @@
         <v>275</v>
       </c>
       <c r="B7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -911,10 +929,10 @@
         <v>277</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -923,10 +941,10 @@
         <v>278</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>3</v>
+        <v>131</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -935,10 +953,10 @@
         <v>279</v>
       </c>
       <c r="B11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" t="s">
         <v>12</v>
-      </c>
-      <c r="C11" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -947,10 +965,10 @@
         <v>280</v>
       </c>
       <c r="B12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C12" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -959,10 +977,10 @@
         <v>281</v>
       </c>
       <c r="B13" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C13" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -971,10 +989,10 @@
         <v>282</v>
       </c>
       <c r="B14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C14" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -983,10 +1001,10 @@
         <v>283</v>
       </c>
       <c r="B15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C15" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -995,10 +1013,10 @@
         <v>284</v>
       </c>
       <c r="B16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C16" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -1007,10 +1025,10 @@
         <v>285</v>
       </c>
       <c r="B17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C17" t="s">
-        <v>3</v>
+        <v>131</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -1031,7 +1049,7 @@
         <v>287</v>
       </c>
       <c r="B19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C19" t="s">
         <v>1</v>
@@ -1043,10 +1061,10 @@
         <v>288</v>
       </c>
       <c r="B20" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -1055,10 +1073,10 @@
         <v>289</v>
       </c>
       <c r="B21" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C21" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -1067,10 +1085,10 @@
         <v>290</v>
       </c>
       <c r="B22" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C22" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -1079,10 +1097,10 @@
         <v>291</v>
       </c>
       <c r="B23" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C23" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -1091,10 +1109,10 @@
         <v>292</v>
       </c>
       <c r="B24" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C24" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -1103,10 +1121,10 @@
         <v>293</v>
       </c>
       <c r="B25" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C25" t="s">
-        <v>3</v>
+        <v>131</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -1115,10 +1133,10 @@
         <v>294</v>
       </c>
       <c r="B26" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C26" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -1127,10 +1145,10 @@
         <v>295</v>
       </c>
       <c r="B27" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C27" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -1139,10 +1157,10 @@
         <v>296</v>
       </c>
       <c r="B28" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C28" t="s">
-        <v>3</v>
+        <v>131</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -1151,10 +1169,10 @@
         <v>297</v>
       </c>
       <c r="B29" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C29" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -1163,10 +1181,10 @@
         <v>298</v>
       </c>
       <c r="B30" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C30" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -1175,10 +1193,10 @@
         <v>299</v>
       </c>
       <c r="B31" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C31" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -1187,10 +1205,10 @@
         <v>300</v>
       </c>
       <c r="B32" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C32" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -1199,10 +1217,10 @@
         <v>301</v>
       </c>
       <c r="B33" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C33" t="s">
-        <v>3</v>
+        <v>131</v>
       </c>
     </row>
     <row r="34" spans="1:3">
@@ -1211,7 +1229,7 @@
         <v>302</v>
       </c>
       <c r="B34" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C34" t="s">
         <v>1</v>
@@ -1223,10 +1241,10 @@
         <v>303</v>
       </c>
       <c r="B35" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C35" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="36" spans="1:3">
@@ -1235,10 +1253,10 @@
         <v>304</v>
       </c>
       <c r="B36" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C36" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -1247,10 +1265,10 @@
         <v>305</v>
       </c>
       <c r="B37" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C37" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="38" spans="1:3">
@@ -1259,10 +1277,10 @@
         <v>306</v>
       </c>
       <c r="B38" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C38" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="39" spans="1:3">
@@ -1271,10 +1289,10 @@
         <v>307</v>
       </c>
       <c r="B39" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C39" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="40" spans="1:3">
@@ -1283,10 +1301,10 @@
         <v>308</v>
       </c>
       <c r="B40" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C40" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="41" spans="1:3">
@@ -1295,10 +1313,10 @@
         <v>309</v>
       </c>
       <c r="B41" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C41" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="42" spans="1:3">
@@ -1307,10 +1325,10 @@
         <v>310</v>
       </c>
       <c r="B42" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C42" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="43" spans="1:3">
@@ -1319,10 +1337,10 @@
         <v>311</v>
       </c>
       <c r="B43" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C43" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="44" spans="1:3">
@@ -1331,10 +1349,10 @@
         <v>312</v>
       </c>
       <c r="B44" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C44" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="45" spans="1:3">
@@ -1343,10 +1361,10 @@
         <v>313</v>
       </c>
       <c r="B45" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C45" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="46" spans="1:3">
@@ -1355,10 +1373,10 @@
         <v>314</v>
       </c>
       <c r="B46" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C46" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="47" spans="1:3">
@@ -1367,10 +1385,10 @@
         <v>315</v>
       </c>
       <c r="B47" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C47" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="48" spans="1:3">
@@ -1379,10 +1397,10 @@
         <v>316</v>
       </c>
       <c r="B48" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C48" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="49" spans="1:3">
@@ -1391,10 +1409,10 @@
         <v>317</v>
       </c>
       <c r="B49" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C49" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="50" spans="1:3">
@@ -1403,10 +1421,10 @@
         <v>318</v>
       </c>
       <c r="B50" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C50" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="51" spans="1:3">
@@ -1415,10 +1433,10 @@
         <v>319</v>
       </c>
       <c r="B51" t="s">
+        <v>44</v>
+      </c>
+      <c r="C51" t="s">
         <v>45</v>
-      </c>
-      <c r="C51" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="52" spans="1:3">
@@ -1427,10 +1445,10 @@
         <v>320</v>
       </c>
       <c r="B52" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C52" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="53" spans="1:3">
@@ -1439,10 +1457,10 @@
         <v>321</v>
       </c>
       <c r="B53" t="s">
+        <v>47</v>
+      </c>
+      <c r="C53" t="s">
         <v>48</v>
-      </c>
-      <c r="C53" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="54" spans="1:3">
@@ -1451,10 +1469,10 @@
         <v>322</v>
       </c>
       <c r="B54" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C54" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="55" spans="1:3">
@@ -1463,10 +1481,10 @@
         <v>323</v>
       </c>
       <c r="B55" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C55" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="56" spans="1:3">
@@ -1475,10 +1493,10 @@
         <v>324</v>
       </c>
       <c r="B56" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C56" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="57" spans="1:3">
@@ -1487,10 +1505,10 @@
         <v>325</v>
       </c>
       <c r="B57" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C57" t="s">
-        <v>3</v>
+        <v>131</v>
       </c>
     </row>
     <row r="58" spans="1:3">
@@ -1499,10 +1517,10 @@
         <v>326</v>
       </c>
       <c r="B58" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C58" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="59" spans="1:3">
@@ -1511,10 +1529,10 @@
         <v>327</v>
       </c>
       <c r="B59" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C59" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="60" spans="1:3">
@@ -1523,10 +1541,10 @@
         <v>328</v>
       </c>
       <c r="B60" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C60" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="61" spans="1:3">
@@ -1535,10 +1553,10 @@
         <v>329</v>
       </c>
       <c r="B61" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C61" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="62" spans="1:3">
@@ -1547,10 +1565,10 @@
         <v>330</v>
       </c>
       <c r="B62" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C62" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="63" spans="1:3">
@@ -1571,10 +1589,10 @@
         <v>332</v>
       </c>
       <c r="B64" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C64" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="65" spans="1:3">
@@ -1583,10 +1601,10 @@
         <v>333</v>
       </c>
       <c r="B65" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C65" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="66" spans="1:3">
@@ -1598,7 +1616,7 @@
         <v>2</v>
       </c>
       <c r="C66" t="s">
-        <v>3</v>
+        <v>131</v>
       </c>
     </row>
     <row r="67" spans="1:3">
@@ -1607,10 +1625,10 @@
         <v>335</v>
       </c>
       <c r="B67" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C67" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="68" spans="1:3">
@@ -1619,10 +1637,10 @@
         <v>336</v>
       </c>
       <c r="B68" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C68" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="69" spans="1:3">
@@ -1631,10 +1649,10 @@
         <v>337</v>
       </c>
       <c r="B69" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C69" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="70" spans="1:3">
@@ -1643,10 +1661,10 @@
         <v>338</v>
       </c>
       <c r="B70" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C70" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="71" spans="1:3">
@@ -1655,10 +1673,10 @@
         <v>339</v>
       </c>
       <c r="B71" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C71" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="72" spans="1:3">
@@ -1667,10 +1685,10 @@
         <v>340</v>
       </c>
       <c r="B72" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C72" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="73" spans="1:3">
@@ -1679,10 +1697,10 @@
         <v>341</v>
       </c>
       <c r="B73" t="s">
+        <v>62</v>
+      </c>
+      <c r="C73" t="s">
         <v>63</v>
-      </c>
-      <c r="C73" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="74" spans="1:3">
@@ -1691,10 +1709,10 @@
         <v>342</v>
       </c>
       <c r="B74" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C74" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="75" spans="1:3">
@@ -1703,10 +1721,10 @@
         <v>343</v>
       </c>
       <c r="B75" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C75" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="76" spans="1:3">
@@ -1715,10 +1733,10 @@
         <v>344</v>
       </c>
       <c r="B76" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C76" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="77" spans="1:3">
@@ -1727,10 +1745,10 @@
         <v>345</v>
       </c>
       <c r="B77" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C77" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="78" spans="1:3">
@@ -1739,10 +1757,10 @@
         <v>346</v>
       </c>
       <c r="B78" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C78" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="79" spans="1:3">
@@ -1751,10 +1769,10 @@
         <v>347</v>
       </c>
       <c r="B79" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C79" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="80" spans="1:3">
@@ -1763,10 +1781,10 @@
         <v>348</v>
       </c>
       <c r="B80" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C80" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="81" spans="1:3">
@@ -1775,10 +1793,10 @@
         <v>349</v>
       </c>
       <c r="B81" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C81" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="82" spans="1:3">
@@ -1787,10 +1805,10 @@
         <v>350</v>
       </c>
       <c r="B82" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C82" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="83" spans="1:3">
@@ -1799,10 +1817,10 @@
         <v>351</v>
       </c>
       <c r="B83" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C83" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="84" spans="1:3">
@@ -1811,10 +1829,10 @@
         <v>352</v>
       </c>
       <c r="B84" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C84" t="s">
-        <v>3</v>
+        <v>131</v>
       </c>
     </row>
     <row r="85" spans="1:3">
@@ -1823,10 +1841,10 @@
         <v>353</v>
       </c>
       <c r="B85" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C85" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="86" spans="1:3">
@@ -1835,10 +1853,10 @@
         <v>354</v>
       </c>
       <c r="B86" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C86" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="87" spans="1:3">
@@ -1847,10 +1865,10 @@
         <v>355</v>
       </c>
       <c r="B87" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C87" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="88" spans="1:3">
@@ -1859,10 +1877,10 @@
         <v>356</v>
       </c>
       <c r="B88" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C88" t="s">
-        <v>3</v>
+        <v>131</v>
       </c>
     </row>
     <row r="89" spans="1:3">
@@ -1871,10 +1889,10 @@
         <v>357</v>
       </c>
       <c r="B89" t="s">
+        <v>53</v>
+      </c>
+      <c r="C89" t="s">
         <v>54</v>
-      </c>
-      <c r="C89" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="90" spans="1:3">
@@ -1883,10 +1901,10 @@
         <v>358</v>
       </c>
       <c r="B90" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C90" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="91" spans="1:3">
@@ -1895,10 +1913,10 @@
         <v>359</v>
       </c>
       <c r="B91" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C91" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="92" spans="1:3">
@@ -1907,10 +1925,10 @@
         <v>360</v>
       </c>
       <c r="B92" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C92" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="93" spans="1:3">
@@ -1919,10 +1937,10 @@
         <v>361</v>
       </c>
       <c r="B93" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C93" t="s">
-        <v>3</v>
+        <v>131</v>
       </c>
     </row>
     <row r="94" spans="1:3">
@@ -1931,10 +1949,10 @@
         <v>362</v>
       </c>
       <c r="B94" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C94" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="95" spans="1:3">
@@ -1943,10 +1961,10 @@
         <v>363</v>
       </c>
       <c r="B95" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C95" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="96" spans="1:3">
@@ -1955,10 +1973,10 @@
         <v>364</v>
       </c>
       <c r="B96" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C96" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="97" spans="1:3">
@@ -1967,10 +1985,10 @@
         <v>365</v>
       </c>
       <c r="B97" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C97" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="98" spans="1:3">
@@ -1979,10 +1997,10 @@
         <v>366</v>
       </c>
       <c r="B98" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C98" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="99" spans="1:3">
@@ -1991,10 +2009,10 @@
         <v>367</v>
       </c>
       <c r="B99" t="s">
+        <v>75</v>
+      </c>
+      <c r="C99" t="s">
         <v>76</v>
-      </c>
-      <c r="C99" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="100" spans="1:3">
@@ -2003,10 +2021,10 @@
         <v>368</v>
       </c>
       <c r="B100" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C100" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="101" spans="1:3">
@@ -2015,10 +2033,10 @@
         <v>369</v>
       </c>
       <c r="B101" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C101" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="102" spans="1:3">
@@ -2027,10 +2045,10 @@
         <v>370</v>
       </c>
       <c r="B102" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C102" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="103" spans="1:3">
@@ -2039,10 +2057,10 @@
         <v>371</v>
       </c>
       <c r="B103" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C103" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="104" spans="1:3">
@@ -2051,10 +2069,10 @@
         <v>372</v>
       </c>
       <c r="B104" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C104" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="105" spans="1:3">
@@ -2063,10 +2081,10 @@
         <v>377</v>
       </c>
       <c r="B105" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C105" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="106" spans="1:3">
@@ -2078,7 +2096,7 @@
         <v>2</v>
       </c>
       <c r="C106" t="s">
-        <v>3</v>
+        <v>131</v>
       </c>
     </row>
     <row r="107" spans="1:3">
@@ -2087,10 +2105,10 @@
         <v>379</v>
       </c>
       <c r="B107" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C107" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="108" spans="1:3">
@@ -2099,10 +2117,10 @@
         <v>380</v>
       </c>
       <c r="B108" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C108" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="109" spans="1:3">
@@ -2111,10 +2129,10 @@
         <v>381</v>
       </c>
       <c r="B109" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C109" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="110" spans="1:3">
@@ -2123,10 +2141,10 @@
         <v>382</v>
       </c>
       <c r="B110" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C110" t="s">
-        <v>3</v>
+        <v>131</v>
       </c>
     </row>
     <row r="111" spans="1:3">
@@ -2135,10 +2153,10 @@
         <v>383</v>
       </c>
       <c r="B111" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C111" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="112" spans="1:3">
@@ -2147,10 +2165,10 @@
         <v>384</v>
       </c>
       <c r="B112" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C112" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="113" spans="1:3">
@@ -2159,10 +2177,10 @@
         <v>385</v>
       </c>
       <c r="B113" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C113" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="114" spans="1:3">
@@ -2171,10 +2189,10 @@
         <v>386</v>
       </c>
       <c r="B114" t="s">
+        <v>11</v>
+      </c>
+      <c r="C114" t="s">
         <v>12</v>
-      </c>
-      <c r="C114" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="115" spans="1:3">
@@ -2183,10 +2201,10 @@
         <v>387</v>
       </c>
       <c r="B115" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C115" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="116" spans="1:3">
@@ -2195,10 +2213,10 @@
         <v>388</v>
       </c>
       <c r="B116" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C116" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="117" spans="1:3">
@@ -2207,10 +2225,10 @@
         <v>389</v>
       </c>
       <c r="B117" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C117" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="118" spans="1:3">
@@ -2222,7 +2240,7 @@
         <v>0</v>
       </c>
       <c r="C118" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="119" spans="1:3">
@@ -2231,10 +2249,10 @@
         <v>391</v>
       </c>
       <c r="B119" t="s">
+        <v>84</v>
+      </c>
+      <c r="C119" t="s">
         <v>85</v>
-      </c>
-      <c r="C119" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="120" spans="1:3">
@@ -2243,10 +2261,10 @@
         <v>392</v>
       </c>
       <c r="B120" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C120" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="121" spans="1:3">
@@ -2255,10 +2273,10 @@
         <v>393</v>
       </c>
       <c r="B121" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C121" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="122" spans="1:3">
@@ -2267,10 +2285,10 @@
         <v>394</v>
       </c>
       <c r="B122" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C122" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="123" spans="1:3">
@@ -2279,10 +2297,10 @@
         <v>395</v>
       </c>
       <c r="B123" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C123" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="124" spans="1:3">
@@ -2291,10 +2309,10 @@
         <v>396</v>
       </c>
       <c r="B124" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C124" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="125" spans="1:3">
@@ -2303,10 +2321,10 @@
         <v>397</v>
       </c>
       <c r="B125" t="s">
+        <v>88</v>
+      </c>
+      <c r="C125" t="s">
         <v>89</v>
-      </c>
-      <c r="C125" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="126" spans="1:3">
@@ -2315,10 +2333,10 @@
         <v>398</v>
       </c>
       <c r="B126" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C126" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="127" spans="1:3">
@@ -2327,10 +2345,10 @@
         <v>399</v>
       </c>
       <c r="B127" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C127" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="128" spans="1:3">
@@ -2342,7 +2360,7 @@
         <v>2</v>
       </c>
       <c r="C128" t="s">
-        <v>3</v>
+        <v>131</v>
       </c>
     </row>
     <row r="129" spans="1:3">
@@ -2351,10 +2369,10 @@
         <v>401</v>
       </c>
       <c r="B129" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C129" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="130" spans="1:3">
@@ -2363,10 +2381,10 @@
         <v>402</v>
       </c>
       <c r="B130" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C130" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="131" spans="1:3">
@@ -2375,10 +2393,10 @@
         <v>403</v>
       </c>
       <c r="B131" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C131" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="132" spans="1:3">
@@ -2387,10 +2405,10 @@
         <v>404</v>
       </c>
       <c r="B132" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C132" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="133" spans="1:3">
@@ -2399,10 +2417,10 @@
         <v>405</v>
       </c>
       <c r="B133" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C133" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="134" spans="1:3">
@@ -2411,10 +2429,10 @@
         <v>406</v>
       </c>
       <c r="B134" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C134" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="135" spans="1:3">
@@ -2423,10 +2441,10 @@
         <v>407</v>
       </c>
       <c r="B135" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C135" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="136" spans="1:3">
@@ -2435,10 +2453,10 @@
         <v>408</v>
       </c>
       <c r="B136" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C136" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="137" spans="1:3">
@@ -2447,10 +2465,10 @@
         <v>409</v>
       </c>
       <c r="B137" t="s">
+        <v>94</v>
+      </c>
+      <c r="C137" t="s">
         <v>95</v>
-      </c>
-      <c r="C137" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="138" spans="1:3">
@@ -2459,10 +2477,10 @@
         <v>410</v>
       </c>
       <c r="B138" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C138" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="139" spans="1:3">
@@ -2471,10 +2489,10 @@
         <v>411</v>
       </c>
       <c r="B139" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C139" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="140" spans="1:3">
@@ -2483,10 +2501,10 @@
         <v>412</v>
       </c>
       <c r="B140" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C140" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="141" spans="1:3">
@@ -2495,10 +2513,10 @@
         <v>413</v>
       </c>
       <c r="B141" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C141" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="142" spans="1:3">
@@ -2507,10 +2525,10 @@
         <v>414</v>
       </c>
       <c r="B142" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C142" t="s">
-        <v>3</v>
+        <v>131</v>
       </c>
     </row>
     <row r="143" spans="1:3">
@@ -2519,10 +2537,10 @@
         <v>415</v>
       </c>
       <c r="B143" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C143" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="144" spans="1:3">
@@ -2531,10 +2549,10 @@
         <v>416</v>
       </c>
       <c r="B144" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C144" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="145" spans="1:3">
@@ -2543,10 +2561,10 @@
         <v>417</v>
       </c>
       <c r="B145" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C145" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="146" spans="1:3">
@@ -2555,10 +2573,10 @@
         <v>418</v>
       </c>
       <c r="B146" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C146" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="147" spans="1:3">
@@ -2567,10 +2585,10 @@
         <v>419</v>
       </c>
       <c r="B147" t="s">
+        <v>102</v>
+      </c>
+      <c r="C147" t="s">
         <v>103</v>
-      </c>
-      <c r="C147" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="148" spans="1:3">
@@ -2579,10 +2597,10 @@
         <v>420</v>
       </c>
       <c r="B148" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C148" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="149" spans="1:3">
@@ -2591,10 +2609,10 @@
         <v>421</v>
       </c>
       <c r="B149" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C149" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="150" spans="1:3">
@@ -2603,10 +2621,10 @@
         <v>422</v>
       </c>
       <c r="B150" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C150" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="151" spans="1:3">
@@ -2615,10 +2633,10 @@
         <v>423</v>
       </c>
       <c r="B151" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C151" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="152" spans="1:3">
@@ -2627,10 +2645,10 @@
         <v>424</v>
       </c>
       <c r="B152" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C152" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="153" spans="1:3">
@@ -2642,7 +2660,7 @@
         <v>2</v>
       </c>
       <c r="C153" t="s">
-        <v>3</v>
+        <v>131</v>
       </c>
     </row>
     <row r="154" spans="1:3">
@@ -2651,10 +2669,10 @@
         <v>426</v>
       </c>
       <c r="B154" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C154" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="155" spans="1:3">
@@ -2663,10 +2681,10 @@
         <v>427</v>
       </c>
       <c r="B155" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C155" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="156" spans="1:3">
@@ -2675,10 +2693,10 @@
         <v>428</v>
       </c>
       <c r="B156" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C156" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="157" spans="1:3">
@@ -2687,10 +2705,10 @@
         <v>429</v>
       </c>
       <c r="B157" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C157" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="158" spans="1:3">
@@ -2699,10 +2717,10 @@
         <v>430</v>
       </c>
       <c r="B158" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C158" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="159" spans="1:3">
@@ -2711,10 +2729,10 @@
         <v>431</v>
       </c>
       <c r="B159" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C159" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="160" spans="1:3">
@@ -2723,10 +2741,10 @@
         <v>432</v>
       </c>
       <c r="B160" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C160" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="161" spans="1:3">
@@ -2738,7 +2756,7 @@
         <v>0</v>
       </c>
       <c r="C161" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="162" spans="1:3">
@@ -2747,10 +2765,10 @@
         <v>434</v>
       </c>
       <c r="B162" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C162" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="163" spans="1:3">
@@ -2759,10 +2777,10 @@
         <v>435</v>
       </c>
       <c r="B163" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C163" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="164" spans="1:3">
@@ -2771,10 +2789,10 @@
         <v>436</v>
       </c>
       <c r="B164" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C164" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="165" spans="1:3">
@@ -2783,10 +2801,10 @@
         <v>437</v>
       </c>
       <c r="B165" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C165" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="166" spans="1:3">
@@ -2795,10 +2813,10 @@
         <v>438</v>
       </c>
       <c r="B166" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C166" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="167" spans="1:3">
@@ -2807,10 +2825,10 @@
         <v>439</v>
       </c>
       <c r="B167" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C167" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="168" spans="1:3">
@@ -2819,10 +2837,10 @@
         <v>440</v>
       </c>
       <c r="B168" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C168" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="169" spans="1:3">
@@ -2831,10 +2849,10 @@
         <v>441</v>
       </c>
       <c r="B169" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C169" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="170" spans="1:3">
@@ -2843,10 +2861,10 @@
         <v>442</v>
       </c>
       <c r="B170" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C170" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="171" spans="1:3">
@@ -2855,10 +2873,10 @@
         <v>443</v>
       </c>
       <c r="B171" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C171" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="172" spans="1:3">
@@ -2867,10 +2885,10 @@
         <v>444</v>
       </c>
       <c r="B172" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C172" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="173" spans="1:3">
@@ -2879,10 +2897,10 @@
         <v>445</v>
       </c>
       <c r="B173" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C173" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="174" spans="1:3">
@@ -2891,10 +2909,10 @@
         <v>446</v>
       </c>
       <c r="B174" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C174" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="175" spans="1:3">
@@ -2903,10 +2921,10 @@
         <v>447</v>
       </c>
       <c r="B175" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C175" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="176" spans="1:3">
@@ -2915,10 +2933,10 @@
         <v>448</v>
       </c>
       <c r="B176" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C176" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="177" spans="1:3">
@@ -2927,10 +2945,10 @@
         <v>449</v>
       </c>
       <c r="B177" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C177" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="178" spans="1:3">
@@ -2942,7 +2960,7 @@
         <v>2</v>
       </c>
       <c r="C178" t="s">
-        <v>3</v>
+        <v>131</v>
       </c>
     </row>
     <row r="179" spans="1:3">
@@ -2951,10 +2969,10 @@
         <v>451</v>
       </c>
       <c r="B179" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C179" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="180" spans="1:3">
@@ -2963,10 +2981,10 @@
         <v>452</v>
       </c>
       <c r="B180" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C180" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="181" spans="1:3">
@@ -2975,10 +2993,10 @@
         <v>453</v>
       </c>
       <c r="B181" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C181" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="182" spans="1:3">
@@ -2987,10 +3005,10 @@
         <v>454</v>
       </c>
       <c r="B182" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C182" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="183" spans="1:3">
@@ -2999,10 +3017,10 @@
         <v>455</v>
       </c>
       <c r="B183" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C183" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="184" spans="1:3">
@@ -3011,10 +3029,10 @@
         <v>456</v>
       </c>
       <c r="B184" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C184" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="185" spans="1:3">
@@ -3023,10 +3041,10 @@
         <v>457</v>
       </c>
       <c r="B185" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C185" t="s">
-        <v>3</v>
+        <v>131</v>
       </c>
     </row>
     <row r="186" spans="1:3">
@@ -3035,10 +3053,10 @@
         <v>458</v>
       </c>
       <c r="B186" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C186" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="187" spans="1:3">
@@ -3047,10 +3065,10 @@
         <v>459</v>
       </c>
       <c r="B187" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C187" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="188" spans="1:3">
@@ -3059,10 +3077,10 @@
         <v>460</v>
       </c>
       <c r="B188" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C188" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="189" spans="1:3">
@@ -3071,10 +3089,10 @@
         <v>461</v>
       </c>
       <c r="B189" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C189" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="190" spans="1:3">
@@ -3083,10 +3101,10 @@
         <v>462</v>
       </c>
       <c r="B190" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C190" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="191" spans="1:3">
@@ -3095,10 +3113,10 @@
         <v>463</v>
       </c>
       <c r="B191" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C191" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="192" spans="1:3">
@@ -3107,10 +3125,10 @@
         <v>464</v>
       </c>
       <c r="B192" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C192" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="193" spans="1:3">
@@ -3119,10 +3137,10 @@
         <v>465</v>
       </c>
       <c r="B193" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C193" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="194" spans="1:3">
@@ -3131,10 +3149,10 @@
         <v>466</v>
       </c>
       <c r="B194" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C194" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="195" spans="1:3">
@@ -3143,10 +3161,10 @@
         <v>467</v>
       </c>
       <c r="B195" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C195" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="196" spans="1:3">
@@ -3155,10 +3173,10 @@
         <v>468</v>
       </c>
       <c r="B196" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C196" t="s">
-        <v>3</v>
+        <v>131</v>
       </c>
     </row>
     <row r="197" spans="1:3">
@@ -3167,10 +3185,10 @@
         <v>469</v>
       </c>
       <c r="B197" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C197" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="198" spans="1:3">
@@ -3179,10 +3197,10 @@
         <v>470</v>
       </c>
       <c r="B198" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C198" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="199" spans="1:3">
@@ -3194,7 +3212,7 @@
         <v>2</v>
       </c>
       <c r="C199" t="s">
-        <v>3</v>
+        <v>131</v>
       </c>
     </row>
     <row r="200" spans="1:3">
@@ -3203,10 +3221,10 @@
         <v>472</v>
       </c>
       <c r="B200" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C200" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="201" spans="1:3">
@@ -3215,10 +3233,10 @@
         <v>473</v>
       </c>
       <c r="B201" t="s">
+        <v>75</v>
+      </c>
+      <c r="C201" t="s">
         <v>76</v>
-      </c>
-      <c r="C201" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="202" spans="1:3">
@@ -3227,10 +3245,10 @@
         <v>474</v>
       </c>
       <c r="B202" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C202" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="203" spans="1:3">
@@ -3239,10 +3257,10 @@
         <v>475</v>
       </c>
       <c r="B203" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C203" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="204" spans="1:3">
@@ -3251,10 +3269,10 @@
         <v>476</v>
       </c>
       <c r="B204" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C204" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="205" spans="1:3">
@@ -3263,10 +3281,10 @@
         <v>477</v>
       </c>
       <c r="B205" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C205" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="206" spans="1:3">
@@ -3275,10 +3293,10 @@
         <v>478</v>
       </c>
       <c r="B206" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C206" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="207" spans="1:3">
@@ -3287,10 +3305,10 @@
         <v>479</v>
       </c>
       <c r="B207" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C207" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="208" spans="1:3">
@@ -3299,10 +3317,10 @@
         <v>480</v>
       </c>
       <c r="B208" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C208" t="s">
-        <v>3</v>
+        <v>131</v>
       </c>
     </row>
     <row r="209" spans="1:3">
@@ -3311,10 +3329,10 @@
         <v>481</v>
       </c>
       <c r="B209" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C209" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="210" spans="1:3">
@@ -3323,10 +3341,10 @@
         <v>482</v>
       </c>
       <c r="B210" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C210" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="211" spans="1:3">
@@ -3335,10 +3353,10 @@
         <v>483</v>
       </c>
       <c r="B211" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C211" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="212" spans="1:3">
@@ -3347,10 +3365,10 @@
         <v>484</v>
       </c>
       <c r="B212" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C212" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="213" spans="1:3">
@@ -3359,10 +3377,10 @@
         <v>485</v>
       </c>
       <c r="B213" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C213" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="214" spans="1:3">
@@ -3371,10 +3389,10 @@
         <v>486</v>
       </c>
       <c r="B214" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C214" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="215" spans="1:3">
@@ -3383,10 +3401,10 @@
         <v>487</v>
       </c>
       <c r="B215" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C215" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="216" spans="1:3">
@@ -3395,10 +3413,10 @@
         <v>488</v>
       </c>
       <c r="B216" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C216" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="217" spans="1:3">
@@ -3407,10 +3425,10 @@
         <v>489</v>
       </c>
       <c r="B217" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C217" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="218" spans="1:3">
@@ -3419,10 +3437,10 @@
         <v>490</v>
       </c>
       <c r="B218" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C218" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="219" spans="1:3">
@@ -3431,10 +3449,10 @@
         <v>491</v>
       </c>
       <c r="B219" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C219" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="220" spans="1:3">
@@ -3443,10 +3461,10 @@
         <v>492</v>
       </c>
       <c r="B220" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C220" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="221" spans="1:3">
@@ -3455,10 +3473,10 @@
         <v>493</v>
       </c>
       <c r="B221" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C221" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="222" spans="1:3">
@@ -3467,10 +3485,10 @@
         <v>494</v>
       </c>
       <c r="B222" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C222" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="223" spans="1:3">
@@ -3479,10 +3497,10 @@
         <v>495</v>
       </c>
       <c r="B223" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C223" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="224" spans="1:3">
@@ -3491,10 +3509,10 @@
         <v>496</v>
       </c>
       <c r="B224" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C224" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="225" spans="1:3">
@@ -3503,10 +3521,10 @@
         <v>497</v>
       </c>
       <c r="B225" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C225" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="226" spans="1:3">
@@ -3515,10 +3533,10 @@
         <v>498</v>
       </c>
       <c r="B226" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C226" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="227" spans="1:3">
@@ -3527,10 +3545,10 @@
         <v>499</v>
       </c>
       <c r="B227" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C227" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="228" spans="1:3">
@@ -3539,10 +3557,10 @@
         <v>500</v>
       </c>
       <c r="B228" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C228" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="229" spans="1:3">
@@ -3551,10 +3569,10 @@
         <v>501</v>
       </c>
       <c r="B229" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C229" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="230" spans="1:3">
@@ -3563,10 +3581,10 @@
         <v>502</v>
       </c>
       <c r="B230" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C230" t="s">
-        <v>3</v>
+        <v>131</v>
       </c>
     </row>
     <row r="231" spans="1:3">
@@ -3575,10 +3593,10 @@
         <v>503</v>
       </c>
       <c r="B231" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C231" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="232" spans="1:3">
@@ -3587,10 +3605,10 @@
         <v>504</v>
       </c>
       <c r="B232" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C232" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="233" spans="1:3">
@@ -3599,10 +3617,10 @@
         <v>505</v>
       </c>
       <c r="B233" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C233" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="234" spans="1:3">
@@ -3611,10 +3629,10 @@
         <v>506</v>
       </c>
       <c r="B234" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C234" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="235" spans="1:3">
@@ -3623,10 +3641,10 @@
         <v>507</v>
       </c>
       <c r="B235" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C235" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="236" spans="1:3">
@@ -3635,10 +3653,10 @@
         <v>508</v>
       </c>
       <c r="B236" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C236" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="237" spans="1:3">
@@ -3647,10 +3665,10 @@
         <v>509</v>
       </c>
       <c r="B237" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C237" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="238" spans="1:3">
@@ -3659,10 +3677,10 @@
         <v>510</v>
       </c>
       <c r="B238" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C238" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="239" spans="1:3">
@@ -3671,10 +3689,10 @@
         <v>511</v>
       </c>
       <c r="B239" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C239" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="240" spans="1:3">
@@ -3686,7 +3704,7 @@
         <v>0</v>
       </c>
       <c r="C240" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="241" spans="1:3">
@@ -3695,10 +3713,10 @@
         <v>513</v>
       </c>
       <c r="B241" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C241" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="242" spans="1:3">
@@ -3707,10 +3725,10 @@
         <v>514</v>
       </c>
       <c r="B242" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C242" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="243" spans="1:3">
@@ -3719,10 +3737,10 @@
         <v>515</v>
       </c>
       <c r="B243" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C243" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="244" spans="1:3">
@@ -3731,10 +3749,10 @@
         <v>516</v>
       </c>
       <c r="B244" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C244" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="245" spans="1:3">
@@ -3743,10 +3761,10 @@
         <v>517</v>
       </c>
       <c r="B245" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C245" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="246" spans="1:3">
@@ -3758,7 +3776,7 @@
         <v>0</v>
       </c>
       <c r="C246" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="247" spans="1:3">
@@ -3767,10 +3785,10 @@
         <v>519</v>
       </c>
       <c r="B247" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C247" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="248" spans="1:3">
@@ -3779,10 +3797,10 @@
         <v>520</v>
       </c>
       <c r="B248" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C248" t="s">
-        <v>3</v>
+        <v>131</v>
       </c>
     </row>
     <row r="249" spans="1:3">
@@ -3791,10 +3809,10 @@
         <v>521</v>
       </c>
       <c r="B249" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C249" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="250" spans="1:3">
@@ -3803,10 +3821,10 @@
         <v>522</v>
       </c>
       <c r="B250" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C250" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="251" spans="1:3">
@@ -3815,10 +3833,10 @@
         <v>523</v>
       </c>
       <c r="B251" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C251" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="252" spans="1:3">
@@ -3827,10 +3845,10 @@
         <v>524</v>
       </c>
       <c r="B252" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C252" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="253" spans="1:3">
@@ -3839,10 +3857,10 @@
         <v>525</v>
       </c>
       <c r="B253" t="s">
+        <v>94</v>
+      </c>
+      <c r="C253" t="s">
         <v>95</v>
-      </c>
-      <c r="C253" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="254" spans="1:3">
@@ -3851,10 +3869,10 @@
         <v>526</v>
       </c>
       <c r="B254" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C254" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="255" spans="1:3">
@@ -3863,10 +3881,10 @@
         <v>527</v>
       </c>
       <c r="B255" t="s">
+        <v>70</v>
+      </c>
+      <c r="C255" t="s">
         <v>71</v>
-      </c>
-      <c r="C255" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="256" spans="1:3">
@@ -3878,7 +3896,7 @@
         <v>2</v>
       </c>
       <c r="C256" t="s">
-        <v>3</v>
+        <v>131</v>
       </c>
     </row>
     <row r="257" spans="1:3">
@@ -3887,10 +3905,10 @@
         <v>529</v>
       </c>
       <c r="B257" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C257" t="s">
-        <v>3</v>
+        <v>131</v>
       </c>
     </row>
     <row r="258" spans="1:3">
@@ -3899,10 +3917,10 @@
         <v>530</v>
       </c>
       <c r="B258" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C258" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="259" spans="1:3">
@@ -3911,10 +3929,10 @@
         <v>531</v>
       </c>
       <c r="B259" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C259" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="260" spans="1:3">
@@ -3923,10 +3941,10 @@
         <v>532</v>
       </c>
       <c r="B260" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C260" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="261" spans="1:3">
@@ -3935,10 +3953,10 @@
         <v>533</v>
       </c>
       <c r="B261" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C261" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="262" spans="1:3">
@@ -3947,10 +3965,10 @@
         <v>534</v>
       </c>
       <c r="B262" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C262" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="263" spans="1:3">
@@ -3959,10 +3977,10 @@
         <v>535</v>
       </c>
       <c r="B263" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C263" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="264" spans="1:3">
@@ -3971,10 +3989,10 @@
         <v>536</v>
       </c>
       <c r="B264" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C264" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="265" spans="1:3">
@@ -3983,10 +4001,10 @@
         <v>537</v>
       </c>
       <c r="B265" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C265" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="266" spans="1:3">
@@ -3995,10 +4013,10 @@
         <v>538</v>
       </c>
       <c r="B266" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C266" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="267" spans="1:3">
@@ -4007,10 +4025,10 @@
         <v>539</v>
       </c>
       <c r="B267" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C267" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="268" spans="1:3">
@@ -4019,10 +4037,10 @@
         <v>540</v>
       </c>
       <c r="B268" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C268" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="269" spans="1:3">
@@ -4031,10 +4049,10 @@
         <v>541</v>
       </c>
       <c r="B269" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C269" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="270" spans="1:3">
@@ -4043,10 +4061,10 @@
         <v>542</v>
       </c>
       <c r="B270" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C270" t="s">
-        <v>3</v>
+        <v>131</v>
       </c>
     </row>
     <row r="271" spans="1:3">
@@ -4055,10 +4073,10 @@
         <v>543</v>
       </c>
       <c r="B271" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C271" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="272" spans="1:3">
@@ -4067,10 +4085,10 @@
         <v>544</v>
       </c>
       <c r="B272" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C272" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="273" spans="1:3">
@@ -4079,10 +4097,10 @@
         <v>545</v>
       </c>
       <c r="B273" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C273" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="274" spans="1:3">
@@ -4091,10 +4109,10 @@
         <v>546</v>
       </c>
       <c r="B274" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C274" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="275" spans="1:3">
@@ -4103,10 +4121,10 @@
         <v>547</v>
       </c>
       <c r="B275" t="s">
+        <v>120</v>
+      </c>
+      <c r="C275" t="s">
         <v>121</v>
-      </c>
-      <c r="C275" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="276" spans="1:3">
@@ -4115,10 +4133,10 @@
         <v>548</v>
       </c>
       <c r="B276" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C276" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="277" spans="1:3">
@@ -4127,10 +4145,10 @@
         <v>549</v>
       </c>
       <c r="B277" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C277" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="278" spans="1:3">
@@ -4139,10 +4157,10 @@
         <v>550</v>
       </c>
       <c r="B278" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C278" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="279" spans="1:3">
@@ -4151,10 +4169,10 @@
         <v>551</v>
       </c>
       <c r="B279" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C279" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="280" spans="1:3">
@@ -4163,10 +4181,10 @@
         <v>552</v>
       </c>
       <c r="B280" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C280" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="281" spans="1:3">
@@ -4175,10 +4193,10 @@
         <v>553</v>
       </c>
       <c r="B281" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C281" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="282" spans="1:3">
@@ -4187,10 +4205,10 @@
         <v>554</v>
       </c>
       <c r="B282" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C282" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="283" spans="1:3">
@@ -4199,10 +4217,10 @@
         <v>555</v>
       </c>
       <c r="B283" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C283" t="s">
-        <v>3</v>
+        <v>131</v>
       </c>
     </row>
     <row r="284" spans="1:3">
@@ -4211,10 +4229,10 @@
         <v>556</v>
       </c>
       <c r="B284" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C284" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="285" spans="1:3">
@@ -4223,10 +4241,10 @@
         <v>557</v>
       </c>
       <c r="B285" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C285" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="286" spans="1:3">
@@ -4235,10 +4253,10 @@
         <v>558</v>
       </c>
       <c r="B286" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C286" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="287" spans="1:3">
@@ -4247,10 +4265,10 @@
         <v>559</v>
       </c>
       <c r="B287" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C287" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="288" spans="1:3">
@@ -4259,10 +4277,10 @@
         <v>560</v>
       </c>
       <c r="B288" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C288" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="289" spans="1:3">
@@ -4271,10 +4289,10 @@
         <v>561</v>
       </c>
       <c r="B289" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C289" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="290" spans="1:3">
@@ -4283,10 +4301,10 @@
         <v>562</v>
       </c>
       <c r="B290" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C290" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="291" spans="1:3">
@@ -4295,10 +4313,10 @@
         <v>563</v>
       </c>
       <c r="B291" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C291" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="292" spans="1:3">
@@ -4307,10 +4325,10 @@
         <v>564</v>
       </c>
       <c r="B292" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C292" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="293" spans="1:3">
@@ -4319,10 +4337,10 @@
         <v>565</v>
       </c>
       <c r="B293" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C293" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="294" spans="1:3">
@@ -4330,10 +4348,10 @@
         <v>566</v>
       </c>
       <c r="B294" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C294" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="295" spans="1:3">
@@ -4341,10 +4359,10 @@
         <v>567</v>
       </c>
       <c r="B295" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C295" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="296" spans="1:3">
@@ -4352,10 +4370,10 @@
         <v>568</v>
       </c>
       <c r="B296" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C296" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="297" spans="1:3">
@@ -4363,10 +4381,10 @@
         <v>569</v>
       </c>
       <c r="B297" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C297" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="298" spans="1:3">
@@ -4374,10 +4392,109 @@
         <v>570</v>
       </c>
       <c r="B298" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C298" t="s">
-        <v>37</v>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="299" spans="1:3">
+      <c r="A299">
+        <v>571</v>
+      </c>
+      <c r="B299" t="s">
+        <v>41</v>
+      </c>
+      <c r="C299" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="300" spans="1:3">
+      <c r="A300">
+        <v>572</v>
+      </c>
+      <c r="B300" t="s">
+        <v>53</v>
+      </c>
+      <c r="C300" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="301" spans="1:3">
+      <c r="A301">
+        <v>573</v>
+      </c>
+      <c r="B301" t="s">
+        <v>57</v>
+      </c>
+      <c r="C301" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="302" spans="1:3">
+      <c r="A302">
+        <v>574</v>
+      </c>
+      <c r="B302" t="s">
+        <v>107</v>
+      </c>
+      <c r="C302" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="303" spans="1:3">
+      <c r="A303">
+        <v>575</v>
+      </c>
+      <c r="B303" t="s">
+        <v>132</v>
+      </c>
+      <c r="C303" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="304" spans="1:3">
+      <c r="A304">
+        <v>576</v>
+      </c>
+      <c r="B304" t="s">
+        <v>55</v>
+      </c>
+      <c r="C304" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="305" spans="1:3">
+      <c r="A305">
+        <v>577</v>
+      </c>
+      <c r="B305" t="s">
+        <v>27</v>
+      </c>
+      <c r="C305" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="306" spans="1:3">
+      <c r="A306">
+        <v>578</v>
+      </c>
+      <c r="B306" t="s">
+        <v>2</v>
+      </c>
+      <c r="C306" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="307" spans="1:3">
+      <c r="A307">
+        <v>579</v>
+      </c>
+      <c r="B307" t="s">
+        <v>7</v>
+      </c>
+      <c r="C307" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated to mission #2194
</commit_message>
<xml_diff>
--- a/Specialist_Mission_BoBs.xlsx
+++ b/Specialist_Mission_BoBs.xlsx
@@ -1,16 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24701"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ortha\Documents\GitHub\BoB-Database\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C55794CF-9FFC-47E3-A593-D22B8D686A6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1300" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Specialist_Mission_BoBs.csv" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -19,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="623" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="729" uniqueCount="143">
   <si>
     <t>Veil</t>
   </si>
@@ -424,12 +439,36 @@
   </si>
   <si>
     <t>JUB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Antioch </t>
+  </si>
+  <si>
+    <t>Cute new dog</t>
+  </si>
+  <si>
+    <t>Starless</t>
+  </si>
+  <si>
+    <t>Mistral</t>
+  </si>
+  <si>
+    <t>Superior</t>
+  </si>
+  <si>
+    <t>Centurion</t>
+  </si>
+  <si>
+    <t>Pastor</t>
+  </si>
+  <si>
+    <t>technically not Flyingfish812 but it probably is Flyingfish812 and I can't be arsed to translate another username that makes literally 0 sense bruh</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -499,6 +538,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -823,16 +870,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C311"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C364"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A282" workbookViewId="0">
-      <selection activeCell="E295" sqref="E295"/>
+    <sheetView tabSelected="1" topLeftCell="A288" workbookViewId="0">
+      <selection activeCell="A312" sqref="A312:C312"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>126</v>
       </c>
@@ -843,7 +890,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>270</v>
       </c>
@@ -854,7 +901,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3">
         <f>A2+1</f>
         <v>271</v>
@@ -866,7 +913,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4">
         <f t="shared" ref="A4:A67" si="0">A3+1</f>
         <v>272</v>
@@ -878,7 +925,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5">
         <f t="shared" si="0"/>
         <v>273</v>
@@ -890,7 +937,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>274</v>
@@ -902,7 +949,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>275</v>
@@ -914,7 +961,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>276</v>
@@ -926,7 +973,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>277</v>
@@ -938,7 +985,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>278</v>
@@ -950,7 +997,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>279</v>
@@ -962,7 +1009,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>280</v>
@@ -974,7 +1021,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13">
         <f t="shared" si="0"/>
         <v>281</v>
@@ -986,7 +1033,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14">
         <f t="shared" si="0"/>
         <v>282</v>
@@ -998,7 +1045,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15">
         <f t="shared" si="0"/>
         <v>283</v>
@@ -1010,7 +1057,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16">
         <f t="shared" si="0"/>
         <v>284</v>
@@ -1022,7 +1069,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17">
         <f t="shared" si="0"/>
         <v>285</v>
@@ -1034,7 +1081,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18">
         <f t="shared" si="0"/>
         <v>286</v>
@@ -1046,7 +1093,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19">
         <f t="shared" si="0"/>
         <v>287</v>
@@ -1058,7 +1105,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20">
         <f t="shared" si="0"/>
         <v>288</v>
@@ -1070,7 +1117,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21">
         <f t="shared" si="0"/>
         <v>289</v>
@@ -1082,7 +1129,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22">
         <f t="shared" si="0"/>
         <v>290</v>
@@ -1094,7 +1141,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23">
         <f t="shared" si="0"/>
         <v>291</v>
@@ -1106,7 +1153,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24">
         <f t="shared" si="0"/>
         <v>292</v>
@@ -1118,7 +1165,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25">
         <f t="shared" si="0"/>
         <v>293</v>
@@ -1130,7 +1177,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26">
         <f t="shared" si="0"/>
         <v>294</v>
@@ -1142,7 +1189,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27">
         <f t="shared" si="0"/>
         <v>295</v>
@@ -1154,7 +1201,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28">
         <f t="shared" si="0"/>
         <v>296</v>
@@ -1166,7 +1213,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29">
         <f t="shared" si="0"/>
         <v>297</v>
@@ -1178,7 +1225,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30">
         <f t="shared" si="0"/>
         <v>298</v>
@@ -1190,7 +1237,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31">
         <f t="shared" si="0"/>
         <v>299</v>
@@ -1202,7 +1249,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32">
         <f t="shared" si="0"/>
         <v>300</v>
@@ -1214,7 +1261,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33">
         <f t="shared" si="0"/>
         <v>301</v>
@@ -1226,7 +1273,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34">
         <f t="shared" si="0"/>
         <v>302</v>
@@ -1238,7 +1285,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35">
         <f t="shared" si="0"/>
         <v>303</v>
@@ -1250,7 +1297,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36">
         <f t="shared" si="0"/>
         <v>304</v>
@@ -1262,7 +1309,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="37" spans="1:3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37">
         <f t="shared" si="0"/>
         <v>305</v>
@@ -1274,7 +1321,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="38" spans="1:3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38">
         <f t="shared" si="0"/>
         <v>306</v>
@@ -1286,7 +1333,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="39" spans="1:3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39">
         <f t="shared" si="0"/>
         <v>307</v>
@@ -1298,7 +1345,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40">
         <f t="shared" si="0"/>
         <v>308</v>
@@ -1310,7 +1357,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="41" spans="1:3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41">
         <f t="shared" si="0"/>
         <v>309</v>
@@ -1322,7 +1369,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="42" spans="1:3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42">
         <f t="shared" si="0"/>
         <v>310</v>
@@ -1334,7 +1381,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="43" spans="1:3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43">
         <f t="shared" si="0"/>
         <v>311</v>
@@ -1346,7 +1393,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="44" spans="1:3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44">
         <f t="shared" si="0"/>
         <v>312</v>
@@ -1358,7 +1405,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="45" spans="1:3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45">
         <f t="shared" si="0"/>
         <v>313</v>
@@ -1370,7 +1417,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="46" spans="1:3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46">
         <f t="shared" si="0"/>
         <v>314</v>
@@ -1382,7 +1429,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="47" spans="1:3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47">
         <f t="shared" si="0"/>
         <v>315</v>
@@ -1394,7 +1441,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="48" spans="1:3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48">
         <f t="shared" si="0"/>
         <v>316</v>
@@ -1406,7 +1453,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="49" spans="1:3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49">
         <f t="shared" si="0"/>
         <v>317</v>
@@ -1418,7 +1465,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="50" spans="1:3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50">
         <f t="shared" si="0"/>
         <v>318</v>
@@ -1430,7 +1477,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="51" spans="1:3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51">
         <f t="shared" si="0"/>
         <v>319</v>
@@ -1442,7 +1489,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="52" spans="1:3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A52">
         <f t="shared" si="0"/>
         <v>320</v>
@@ -1454,7 +1501,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="53" spans="1:3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A53">
         <f t="shared" si="0"/>
         <v>321</v>
@@ -1466,7 +1513,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="54" spans="1:3">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A54">
         <f t="shared" si="0"/>
         <v>322</v>
@@ -1478,7 +1525,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="55" spans="1:3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A55">
         <f t="shared" si="0"/>
         <v>323</v>
@@ -1490,7 +1537,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="56" spans="1:3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A56">
         <f t="shared" si="0"/>
         <v>324</v>
@@ -1502,7 +1549,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="57" spans="1:3">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A57">
         <f t="shared" si="0"/>
         <v>325</v>
@@ -1514,7 +1561,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="58" spans="1:3">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A58">
         <f t="shared" si="0"/>
         <v>326</v>
@@ -1526,7 +1573,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="59" spans="1:3">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A59">
         <f t="shared" si="0"/>
         <v>327</v>
@@ -1538,7 +1585,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="60" spans="1:3">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A60">
         <f t="shared" si="0"/>
         <v>328</v>
@@ -1550,7 +1597,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="61" spans="1:3">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A61">
         <f t="shared" si="0"/>
         <v>329</v>
@@ -1562,7 +1609,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="62" spans="1:3">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A62">
         <f t="shared" si="0"/>
         <v>330</v>
@@ -1574,7 +1621,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="63" spans="1:3">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A63">
         <f t="shared" si="0"/>
         <v>331</v>
@@ -1586,7 +1633,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:3">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A64">
         <f t="shared" si="0"/>
         <v>332</v>
@@ -1598,7 +1645,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="65" spans="1:3">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A65">
         <f t="shared" si="0"/>
         <v>333</v>
@@ -1610,7 +1657,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="66" spans="1:3">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A66">
         <f t="shared" si="0"/>
         <v>334</v>
@@ -1622,7 +1669,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="67" spans="1:3">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A67">
         <f t="shared" si="0"/>
         <v>335</v>
@@ -1634,7 +1681,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="68" spans="1:3">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A68">
         <f t="shared" ref="A68:A104" si="1">A67+1</f>
         <v>336</v>
@@ -1646,7 +1693,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="69" spans="1:3">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A69">
         <f t="shared" si="1"/>
         <v>337</v>
@@ -1658,7 +1705,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="70" spans="1:3">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A70">
         <f t="shared" si="1"/>
         <v>338</v>
@@ -1670,7 +1717,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="71" spans="1:3">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A71">
         <f t="shared" si="1"/>
         <v>339</v>
@@ -1682,7 +1729,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="72" spans="1:3">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A72">
         <f t="shared" si="1"/>
         <v>340</v>
@@ -1694,7 +1741,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="73" spans="1:3">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A73">
         <f t="shared" si="1"/>
         <v>341</v>
@@ -1706,7 +1753,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="74" spans="1:3">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A74">
         <f t="shared" si="1"/>
         <v>342</v>
@@ -1718,7 +1765,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="75" spans="1:3">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A75">
         <f t="shared" si="1"/>
         <v>343</v>
@@ -1730,7 +1777,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="76" spans="1:3">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A76">
         <f t="shared" si="1"/>
         <v>344</v>
@@ -1742,7 +1789,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="77" spans="1:3">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A77">
         <f t="shared" si="1"/>
         <v>345</v>
@@ -1754,7 +1801,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="78" spans="1:3">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A78">
         <f t="shared" si="1"/>
         <v>346</v>
@@ -1766,7 +1813,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="79" spans="1:3">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A79">
         <f t="shared" si="1"/>
         <v>347</v>
@@ -1778,7 +1825,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="80" spans="1:3">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A80">
         <f t="shared" si="1"/>
         <v>348</v>
@@ -1790,7 +1837,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="81" spans="1:3">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A81">
         <f t="shared" si="1"/>
         <v>349</v>
@@ -1802,7 +1849,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="82" spans="1:3">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A82">
         <f t="shared" si="1"/>
         <v>350</v>
@@ -1814,7 +1861,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="83" spans="1:3">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A83">
         <f t="shared" si="1"/>
         <v>351</v>
@@ -1826,7 +1873,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="84" spans="1:3">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A84">
         <f t="shared" si="1"/>
         <v>352</v>
@@ -1838,7 +1885,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="85" spans="1:3">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A85">
         <f t="shared" si="1"/>
         <v>353</v>
@@ -1850,7 +1897,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="86" spans="1:3">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A86">
         <f t="shared" si="1"/>
         <v>354</v>
@@ -1862,7 +1909,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="87" spans="1:3">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A87">
         <f t="shared" si="1"/>
         <v>355</v>
@@ -1874,7 +1921,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="88" spans="1:3">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A88">
         <f t="shared" si="1"/>
         <v>356</v>
@@ -1886,7 +1933,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="89" spans="1:3">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A89">
         <f t="shared" si="1"/>
         <v>357</v>
@@ -1898,7 +1945,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="90" spans="1:3">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A90">
         <f t="shared" si="1"/>
         <v>358</v>
@@ -1910,7 +1957,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="91" spans="1:3">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A91">
         <f t="shared" si="1"/>
         <v>359</v>
@@ -1922,7 +1969,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="92" spans="1:3">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A92">
         <f t="shared" si="1"/>
         <v>360</v>
@@ -1934,7 +1981,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="93" spans="1:3">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A93">
         <f t="shared" si="1"/>
         <v>361</v>
@@ -1946,7 +1993,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="94" spans="1:3">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A94">
         <f t="shared" si="1"/>
         <v>362</v>
@@ -1958,7 +2005,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="95" spans="1:3">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A95">
         <f t="shared" si="1"/>
         <v>363</v>
@@ -1970,7 +2017,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="96" spans="1:3">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A96">
         <f t="shared" si="1"/>
         <v>364</v>
@@ -1982,7 +2029,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="97" spans="1:3">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A97">
         <f t="shared" si="1"/>
         <v>365</v>
@@ -1994,7 +2041,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="98" spans="1:3">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A98">
         <f t="shared" si="1"/>
         <v>366</v>
@@ -2006,7 +2053,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="99" spans="1:3">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A99">
         <f t="shared" si="1"/>
         <v>367</v>
@@ -2018,7 +2065,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="100" spans="1:3">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A100">
         <f t="shared" si="1"/>
         <v>368</v>
@@ -2030,7 +2077,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="101" spans="1:3">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A101">
         <f t="shared" si="1"/>
         <v>369</v>
@@ -2042,7 +2089,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="102" spans="1:3">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A102">
         <f t="shared" si="1"/>
         <v>370</v>
@@ -2054,7 +2101,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="103" spans="1:3">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A103">
         <f t="shared" si="1"/>
         <v>371</v>
@@ -2066,7 +2113,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="104" spans="1:3">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A104">
         <f t="shared" si="1"/>
         <v>372</v>
@@ -2078,7 +2125,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="105" spans="1:3">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A105">
         <f>A104+5</f>
         <v>377</v>
@@ -2090,7 +2137,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="106" spans="1:3">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A106">
         <f t="shared" ref="A106:A127" si="2">A105+1</f>
         <v>378</v>
@@ -2102,7 +2149,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="107" spans="1:3">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A107">
         <f t="shared" si="2"/>
         <v>379</v>
@@ -2114,7 +2161,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="108" spans="1:3">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A108">
         <f t="shared" si="2"/>
         <v>380</v>
@@ -2126,7 +2173,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="109" spans="1:3">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A109">
         <f t="shared" si="2"/>
         <v>381</v>
@@ -2138,7 +2185,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="110" spans="1:3">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A110">
         <f t="shared" si="2"/>
         <v>382</v>
@@ -2150,7 +2197,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="111" spans="1:3">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A111">
         <f t="shared" si="2"/>
         <v>383</v>
@@ -2162,7 +2209,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="112" spans="1:3">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A112">
         <f t="shared" si="2"/>
         <v>384</v>
@@ -2174,7 +2221,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="113" spans="1:3">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A113">
         <f t="shared" si="2"/>
         <v>385</v>
@@ -2186,7 +2233,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="114" spans="1:3">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A114">
         <f t="shared" si="2"/>
         <v>386</v>
@@ -2198,7 +2245,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="115" spans="1:3">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A115">
         <f t="shared" si="2"/>
         <v>387</v>
@@ -2210,7 +2257,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="116" spans="1:3">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A116">
         <f t="shared" si="2"/>
         <v>388</v>
@@ -2222,7 +2269,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="117" spans="1:3">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A117">
         <f t="shared" si="2"/>
         <v>389</v>
@@ -2234,7 +2281,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="118" spans="1:3">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A118">
         <f t="shared" si="2"/>
         <v>390</v>
@@ -2246,7 +2293,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="119" spans="1:3">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A119">
         <f t="shared" si="2"/>
         <v>391</v>
@@ -2258,7 +2305,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="120" spans="1:3">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A120">
         <f t="shared" si="2"/>
         <v>392</v>
@@ -2270,7 +2317,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="121" spans="1:3">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A121">
         <f t="shared" si="2"/>
         <v>393</v>
@@ -2282,7 +2329,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="122" spans="1:3">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A122">
         <f t="shared" si="2"/>
         <v>394</v>
@@ -2294,7 +2341,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="123" spans="1:3">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A123">
         <f t="shared" si="2"/>
         <v>395</v>
@@ -2306,7 +2353,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="124" spans="1:3">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A124">
         <f t="shared" si="2"/>
         <v>396</v>
@@ -2318,7 +2365,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="125" spans="1:3">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A125">
         <f t="shared" si="2"/>
         <v>397</v>
@@ -2330,7 +2377,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="126" spans="1:3">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A126">
         <f t="shared" si="2"/>
         <v>398</v>
@@ -2342,7 +2389,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="127" spans="1:3">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A127">
         <f t="shared" si="2"/>
         <v>399</v>
@@ -2354,7 +2401,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="128" spans="1:3">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A128">
         <f t="shared" ref="A128:A169" si="3">A127+1</f>
         <v>400</v>
@@ -2366,7 +2413,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="129" spans="1:3">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A129">
         <f t="shared" si="3"/>
         <v>401</v>
@@ -2378,7 +2425,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="130" spans="1:3">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A130">
         <f t="shared" si="3"/>
         <v>402</v>
@@ -2390,7 +2437,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="131" spans="1:3">
+    <row r="131" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A131">
         <f t="shared" si="3"/>
         <v>403</v>
@@ -2402,7 +2449,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="132" spans="1:3">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A132">
         <f t="shared" si="3"/>
         <v>404</v>
@@ -2414,7 +2461,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="133" spans="1:3">
+    <row r="133" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A133">
         <f t="shared" si="3"/>
         <v>405</v>
@@ -2426,7 +2473,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="134" spans="1:3">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A134">
         <f t="shared" si="3"/>
         <v>406</v>
@@ -2438,7 +2485,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="135" spans="1:3">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A135">
         <f t="shared" si="3"/>
         <v>407</v>
@@ -2450,7 +2497,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="136" spans="1:3">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A136">
         <f t="shared" si="3"/>
         <v>408</v>
@@ -2462,7 +2509,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="137" spans="1:3">
+    <row r="137" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A137">
         <f t="shared" si="3"/>
         <v>409</v>
@@ -2474,7 +2521,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="138" spans="1:3">
+    <row r="138" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A138">
         <f t="shared" si="3"/>
         <v>410</v>
@@ -2486,7 +2533,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="139" spans="1:3">
+    <row r="139" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A139">
         <f t="shared" si="3"/>
         <v>411</v>
@@ -2498,7 +2545,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="140" spans="1:3">
+    <row r="140" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A140">
         <f t="shared" si="3"/>
         <v>412</v>
@@ -2510,7 +2557,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="141" spans="1:3">
+    <row r="141" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A141">
         <f t="shared" si="3"/>
         <v>413</v>
@@ -2522,7 +2569,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="142" spans="1:3">
+    <row r="142" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A142">
         <f t="shared" si="3"/>
         <v>414</v>
@@ -2534,7 +2581,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="143" spans="1:3">
+    <row r="143" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A143">
         <f t="shared" si="3"/>
         <v>415</v>
@@ -2546,7 +2593,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="144" spans="1:3">
+    <row r="144" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A144">
         <f t="shared" si="3"/>
         <v>416</v>
@@ -2558,7 +2605,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="145" spans="1:3">
+    <row r="145" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A145">
         <f t="shared" si="3"/>
         <v>417</v>
@@ -2570,7 +2617,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="146" spans="1:3">
+    <row r="146" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A146">
         <f t="shared" si="3"/>
         <v>418</v>
@@ -2582,7 +2629,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="147" spans="1:3">
+    <row r="147" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A147">
         <f t="shared" si="3"/>
         <v>419</v>
@@ -2594,7 +2641,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="148" spans="1:3">
+    <row r="148" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A148">
         <f t="shared" si="3"/>
         <v>420</v>
@@ -2606,7 +2653,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="149" spans="1:3">
+    <row r="149" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A149">
         <f t="shared" si="3"/>
         <v>421</v>
@@ -2618,7 +2665,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="150" spans="1:3">
+    <row r="150" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A150">
         <f t="shared" si="3"/>
         <v>422</v>
@@ -2630,7 +2677,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="151" spans="1:3">
+    <row r="151" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A151">
         <f t="shared" si="3"/>
         <v>423</v>
@@ -2642,7 +2689,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="152" spans="1:3">
+    <row r="152" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A152">
         <f t="shared" si="3"/>
         <v>424</v>
@@ -2654,7 +2701,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="153" spans="1:3">
+    <row r="153" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A153">
         <f t="shared" si="3"/>
         <v>425</v>
@@ -2666,7 +2713,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="154" spans="1:3">
+    <row r="154" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A154">
         <f t="shared" si="3"/>
         <v>426</v>
@@ -2678,7 +2725,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="155" spans="1:3">
+    <row r="155" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A155">
         <f t="shared" si="3"/>
         <v>427</v>
@@ -2690,7 +2737,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="156" spans="1:3">
+    <row r="156" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A156">
         <f t="shared" si="3"/>
         <v>428</v>
@@ -2702,7 +2749,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="157" spans="1:3">
+    <row r="157" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A157">
         <f t="shared" si="3"/>
         <v>429</v>
@@ -2714,7 +2761,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="158" spans="1:3">
+    <row r="158" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A158">
         <f t="shared" si="3"/>
         <v>430</v>
@@ -2726,7 +2773,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="159" spans="1:3">
+    <row r="159" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A159">
         <f t="shared" si="3"/>
         <v>431</v>
@@ -2738,7 +2785,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="160" spans="1:3">
+    <row r="160" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A160">
         <f t="shared" si="3"/>
         <v>432</v>
@@ -2750,7 +2797,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="161" spans="1:3">
+    <row r="161" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A161">
         <f t="shared" si="3"/>
         <v>433</v>
@@ -2762,7 +2809,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="162" spans="1:3">
+    <row r="162" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A162">
         <f t="shared" si="3"/>
         <v>434</v>
@@ -2774,7 +2821,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="163" spans="1:3">
+    <row r="163" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A163">
         <f t="shared" si="3"/>
         <v>435</v>
@@ -2786,7 +2833,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="164" spans="1:3">
+    <row r="164" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A164">
         <f t="shared" si="3"/>
         <v>436</v>
@@ -2798,7 +2845,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="165" spans="1:3">
+    <row r="165" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A165">
         <f t="shared" si="3"/>
         <v>437</v>
@@ -2810,7 +2857,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="166" spans="1:3">
+    <row r="166" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A166">
         <f t="shared" si="3"/>
         <v>438</v>
@@ -2822,7 +2869,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="167" spans="1:3">
+    <row r="167" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A167">
         <f t="shared" si="3"/>
         <v>439</v>
@@ -2834,7 +2881,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="168" spans="1:3">
+    <row r="168" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A168">
         <f t="shared" si="3"/>
         <v>440</v>
@@ -2846,7 +2893,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="169" spans="1:3">
+    <row r="169" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A169">
         <f t="shared" si="3"/>
         <v>441</v>
@@ -2858,7 +2905,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="170" spans="1:3">
+    <row r="170" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A170">
         <f>A169+1</f>
         <v>442</v>
@@ -2870,7 +2917,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="171" spans="1:3">
+    <row r="171" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A171">
         <f t="shared" ref="A171:A234" si="4">A170+1</f>
         <v>443</v>
@@ -2882,7 +2929,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="172" spans="1:3">
+    <row r="172" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A172">
         <f t="shared" si="4"/>
         <v>444</v>
@@ -2894,7 +2941,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="173" spans="1:3">
+    <row r="173" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A173">
         <f t="shared" si="4"/>
         <v>445</v>
@@ -2906,7 +2953,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="174" spans="1:3">
+    <row r="174" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A174">
         <f t="shared" si="4"/>
         <v>446</v>
@@ -2918,7 +2965,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="175" spans="1:3">
+    <row r="175" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A175">
         <f t="shared" si="4"/>
         <v>447</v>
@@ -2930,7 +2977,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="176" spans="1:3">
+    <row r="176" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A176">
         <f t="shared" si="4"/>
         <v>448</v>
@@ -2942,7 +2989,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="177" spans="1:3">
+    <row r="177" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A177">
         <f t="shared" si="4"/>
         <v>449</v>
@@ -2954,7 +3001,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="178" spans="1:3">
+    <row r="178" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A178">
         <f t="shared" si="4"/>
         <v>450</v>
@@ -2966,7 +3013,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="179" spans="1:3">
+    <row r="179" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A179">
         <f t="shared" si="4"/>
         <v>451</v>
@@ -2978,7 +3025,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="180" spans="1:3">
+    <row r="180" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A180">
         <f t="shared" si="4"/>
         <v>452</v>
@@ -2990,7 +3037,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="181" spans="1:3">
+    <row r="181" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A181">
         <f t="shared" si="4"/>
         <v>453</v>
@@ -3002,7 +3049,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="182" spans="1:3">
+    <row r="182" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A182">
         <f t="shared" si="4"/>
         <v>454</v>
@@ -3014,7 +3061,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="183" spans="1:3">
+    <row r="183" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A183">
         <f t="shared" si="4"/>
         <v>455</v>
@@ -3026,7 +3073,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="184" spans="1:3">
+    <row r="184" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A184">
         <f t="shared" si="4"/>
         <v>456</v>
@@ -3038,7 +3085,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="185" spans="1:3">
+    <row r="185" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A185">
         <f t="shared" si="4"/>
         <v>457</v>
@@ -3050,7 +3097,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="186" spans="1:3">
+    <row r="186" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A186">
         <f t="shared" si="4"/>
         <v>458</v>
@@ -3062,7 +3109,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="187" spans="1:3">
+    <row r="187" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A187">
         <f t="shared" si="4"/>
         <v>459</v>
@@ -3074,7 +3121,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="188" spans="1:3">
+    <row r="188" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A188">
         <f t="shared" si="4"/>
         <v>460</v>
@@ -3086,7 +3133,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="189" spans="1:3">
+    <row r="189" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A189">
         <f t="shared" si="4"/>
         <v>461</v>
@@ -3098,7 +3145,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="190" spans="1:3">
+    <row r="190" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A190">
         <f t="shared" si="4"/>
         <v>462</v>
@@ -3110,7 +3157,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="191" spans="1:3">
+    <row r="191" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A191">
         <f t="shared" si="4"/>
         <v>463</v>
@@ -3122,7 +3169,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="192" spans="1:3">
+    <row r="192" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A192">
         <f t="shared" si="4"/>
         <v>464</v>
@@ -3134,7 +3181,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="193" spans="1:3">
+    <row r="193" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A193">
         <f t="shared" si="4"/>
         <v>465</v>
@@ -3146,7 +3193,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="194" spans="1:3">
+    <row r="194" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A194">
         <f t="shared" si="4"/>
         <v>466</v>
@@ -3158,7 +3205,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="195" spans="1:3">
+    <row r="195" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A195">
         <f t="shared" si="4"/>
         <v>467</v>
@@ -3170,7 +3217,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="196" spans="1:3">
+    <row r="196" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A196">
         <f t="shared" si="4"/>
         <v>468</v>
@@ -3182,7 +3229,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="197" spans="1:3">
+    <row r="197" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A197">
         <f t="shared" si="4"/>
         <v>469</v>
@@ -3194,7 +3241,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="198" spans="1:3">
+    <row r="198" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A198">
         <f t="shared" si="4"/>
         <v>470</v>
@@ -3206,7 +3253,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="199" spans="1:3">
+    <row r="199" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A199">
         <f t="shared" si="4"/>
         <v>471</v>
@@ -3218,7 +3265,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="200" spans="1:3">
+    <row r="200" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A200">
         <f t="shared" si="4"/>
         <v>472</v>
@@ -3230,7 +3277,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="201" spans="1:3">
+    <row r="201" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A201">
         <f t="shared" si="4"/>
         <v>473</v>
@@ -3242,7 +3289,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="202" spans="1:3">
+    <row r="202" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A202">
         <f t="shared" si="4"/>
         <v>474</v>
@@ -3254,7 +3301,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="203" spans="1:3">
+    <row r="203" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A203">
         <f t="shared" si="4"/>
         <v>475</v>
@@ -3266,7 +3313,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="204" spans="1:3">
+    <row r="204" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A204">
         <f t="shared" si="4"/>
         <v>476</v>
@@ -3278,7 +3325,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="205" spans="1:3">
+    <row r="205" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A205">
         <f t="shared" si="4"/>
         <v>477</v>
@@ -3290,7 +3337,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="206" spans="1:3">
+    <row r="206" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A206">
         <f t="shared" si="4"/>
         <v>478</v>
@@ -3302,7 +3349,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="207" spans="1:3">
+    <row r="207" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A207">
         <f t="shared" si="4"/>
         <v>479</v>
@@ -3314,7 +3361,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="208" spans="1:3">
+    <row r="208" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A208">
         <f t="shared" si="4"/>
         <v>480</v>
@@ -3326,7 +3373,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="209" spans="1:3">
+    <row r="209" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A209">
         <f t="shared" si="4"/>
         <v>481</v>
@@ -3338,7 +3385,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="210" spans="1:3">
+    <row r="210" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A210">
         <f t="shared" si="4"/>
         <v>482</v>
@@ -3350,7 +3397,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="211" spans="1:3">
+    <row r="211" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A211">
         <f t="shared" si="4"/>
         <v>483</v>
@@ -3362,7 +3409,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="212" spans="1:3">
+    <row r="212" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A212">
         <f t="shared" si="4"/>
         <v>484</v>
@@ -3374,7 +3421,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="213" spans="1:3">
+    <row r="213" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A213">
         <f t="shared" si="4"/>
         <v>485</v>
@@ -3386,7 +3433,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="214" spans="1:3">
+    <row r="214" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A214">
         <f t="shared" si="4"/>
         <v>486</v>
@@ -3398,7 +3445,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="215" spans="1:3">
+    <row r="215" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A215">
         <f t="shared" si="4"/>
         <v>487</v>
@@ -3410,7 +3457,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="216" spans="1:3">
+    <row r="216" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A216">
         <f t="shared" si="4"/>
         <v>488</v>
@@ -3422,7 +3469,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="217" spans="1:3">
+    <row r="217" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A217">
         <f t="shared" si="4"/>
         <v>489</v>
@@ -3434,7 +3481,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="218" spans="1:3">
+    <row r="218" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A218">
         <f t="shared" si="4"/>
         <v>490</v>
@@ -3446,7 +3493,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="219" spans="1:3">
+    <row r="219" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A219">
         <f t="shared" si="4"/>
         <v>491</v>
@@ -3458,7 +3505,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="220" spans="1:3">
+    <row r="220" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A220">
         <f t="shared" si="4"/>
         <v>492</v>
@@ -3470,7 +3517,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="221" spans="1:3">
+    <row r="221" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A221">
         <f t="shared" si="4"/>
         <v>493</v>
@@ -3482,7 +3529,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="222" spans="1:3">
+    <row r="222" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A222">
         <f t="shared" si="4"/>
         <v>494</v>
@@ -3494,7 +3541,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="223" spans="1:3">
+    <row r="223" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A223">
         <f t="shared" si="4"/>
         <v>495</v>
@@ -3506,7 +3553,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="224" spans="1:3">
+    <row r="224" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A224">
         <f t="shared" si="4"/>
         <v>496</v>
@@ -3518,7 +3565,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="225" spans="1:3">
+    <row r="225" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A225">
         <f t="shared" si="4"/>
         <v>497</v>
@@ -3530,7 +3577,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="226" spans="1:3">
+    <row r="226" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A226">
         <f t="shared" si="4"/>
         <v>498</v>
@@ -3542,7 +3589,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="227" spans="1:3">
+    <row r="227" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A227">
         <f t="shared" si="4"/>
         <v>499</v>
@@ -3554,7 +3601,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="228" spans="1:3">
+    <row r="228" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A228">
         <f t="shared" si="4"/>
         <v>500</v>
@@ -3566,7 +3613,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="229" spans="1:3">
+    <row r="229" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A229">
         <f t="shared" si="4"/>
         <v>501</v>
@@ -3578,7 +3625,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="230" spans="1:3">
+    <row r="230" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A230">
         <f t="shared" si="4"/>
         <v>502</v>
@@ -3590,7 +3637,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="231" spans="1:3">
+    <row r="231" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A231">
         <f t="shared" si="4"/>
         <v>503</v>
@@ -3602,7 +3649,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="232" spans="1:3">
+    <row r="232" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A232">
         <f t="shared" si="4"/>
         <v>504</v>
@@ -3614,7 +3661,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="233" spans="1:3">
+    <row r="233" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A233">
         <f t="shared" si="4"/>
         <v>505</v>
@@ -3626,7 +3673,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="234" spans="1:3">
+    <row r="234" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A234">
         <f t="shared" si="4"/>
         <v>506</v>
@@ -3638,7 +3685,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="235" spans="1:3">
+    <row r="235" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A235">
         <f t="shared" ref="A235:A293" si="5">A234+1</f>
         <v>507</v>
@@ -3650,7 +3697,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="236" spans="1:3">
+    <row r="236" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A236">
         <f t="shared" si="5"/>
         <v>508</v>
@@ -3662,7 +3709,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="237" spans="1:3">
+    <row r="237" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A237">
         <f t="shared" si="5"/>
         <v>509</v>
@@ -3674,7 +3721,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="238" spans="1:3">
+    <row r="238" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A238">
         <f t="shared" si="5"/>
         <v>510</v>
@@ -3686,7 +3733,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="239" spans="1:3">
+    <row r="239" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A239">
         <f t="shared" si="5"/>
         <v>511</v>
@@ -3698,7 +3745,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="240" spans="1:3">
+    <row r="240" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A240">
         <f t="shared" si="5"/>
         <v>512</v>
@@ -3710,7 +3757,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="241" spans="1:3">
+    <row r="241" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A241">
         <f t="shared" si="5"/>
         <v>513</v>
@@ -3722,7 +3769,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="242" spans="1:3">
+    <row r="242" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A242">
         <f t="shared" si="5"/>
         <v>514</v>
@@ -3734,7 +3781,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="243" spans="1:3">
+    <row r="243" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A243">
         <f t="shared" si="5"/>
         <v>515</v>
@@ -3746,7 +3793,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="244" spans="1:3">
+    <row r="244" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A244">
         <f t="shared" si="5"/>
         <v>516</v>
@@ -3758,7 +3805,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="245" spans="1:3">
+    <row r="245" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A245">
         <f t="shared" si="5"/>
         <v>517</v>
@@ -3770,7 +3817,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="246" spans="1:3">
+    <row r="246" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A246">
         <f t="shared" si="5"/>
         <v>518</v>
@@ -3782,7 +3829,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="247" spans="1:3">
+    <row r="247" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A247">
         <f t="shared" si="5"/>
         <v>519</v>
@@ -3794,7 +3841,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="248" spans="1:3">
+    <row r="248" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A248">
         <f t="shared" si="5"/>
         <v>520</v>
@@ -3806,7 +3853,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="249" spans="1:3">
+    <row r="249" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A249">
         <f t="shared" si="5"/>
         <v>521</v>
@@ -3818,7 +3865,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="250" spans="1:3">
+    <row r="250" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A250">
         <f t="shared" si="5"/>
         <v>522</v>
@@ -3830,7 +3877,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="251" spans="1:3">
+    <row r="251" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A251">
         <f t="shared" si="5"/>
         <v>523</v>
@@ -3842,7 +3889,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="252" spans="1:3">
+    <row r="252" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A252">
         <f t="shared" si="5"/>
         <v>524</v>
@@ -3854,7 +3901,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="253" spans="1:3">
+    <row r="253" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A253">
         <f t="shared" si="5"/>
         <v>525</v>
@@ -3866,7 +3913,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="254" spans="1:3">
+    <row r="254" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A254">
         <f t="shared" si="5"/>
         <v>526</v>
@@ -3878,7 +3925,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="255" spans="1:3">
+    <row r="255" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A255">
         <f t="shared" si="5"/>
         <v>527</v>
@@ -3890,7 +3937,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="256" spans="1:3">
+    <row r="256" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A256">
         <f t="shared" si="5"/>
         <v>528</v>
@@ -3902,7 +3949,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="257" spans="1:3">
+    <row r="257" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A257">
         <f t="shared" si="5"/>
         <v>529</v>
@@ -3914,7 +3961,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="258" spans="1:3">
+    <row r="258" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A258">
         <f t="shared" si="5"/>
         <v>530</v>
@@ -3926,7 +3973,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="259" spans="1:3">
+    <row r="259" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A259">
         <f t="shared" si="5"/>
         <v>531</v>
@@ -3938,7 +3985,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="260" spans="1:3">
+    <row r="260" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A260">
         <f t="shared" si="5"/>
         <v>532</v>
@@ -3950,7 +3997,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="261" spans="1:3">
+    <row r="261" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A261">
         <f t="shared" si="5"/>
         <v>533</v>
@@ -3962,7 +4009,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="262" spans="1:3">
+    <row r="262" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A262">
         <f t="shared" si="5"/>
         <v>534</v>
@@ -3974,7 +4021,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="263" spans="1:3">
+    <row r="263" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A263">
         <f t="shared" si="5"/>
         <v>535</v>
@@ -3986,7 +4033,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="264" spans="1:3">
+    <row r="264" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A264">
         <f t="shared" si="5"/>
         <v>536</v>
@@ -3998,7 +4045,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="265" spans="1:3">
+    <row r="265" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A265">
         <f t="shared" si="5"/>
         <v>537</v>
@@ -4010,7 +4057,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="266" spans="1:3">
+    <row r="266" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A266">
         <f t="shared" si="5"/>
         <v>538</v>
@@ -4022,7 +4069,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="267" spans="1:3">
+    <row r="267" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A267">
         <f t="shared" si="5"/>
         <v>539</v>
@@ -4034,7 +4081,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="268" spans="1:3">
+    <row r="268" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A268">
         <f t="shared" si="5"/>
         <v>540</v>
@@ -4046,7 +4093,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="269" spans="1:3">
+    <row r="269" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A269">
         <f t="shared" si="5"/>
         <v>541</v>
@@ -4058,7 +4105,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="270" spans="1:3">
+    <row r="270" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A270">
         <f t="shared" si="5"/>
         <v>542</v>
@@ -4070,7 +4117,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="271" spans="1:3">
+    <row r="271" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A271">
         <f t="shared" si="5"/>
         <v>543</v>
@@ -4082,7 +4129,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="272" spans="1:3">
+    <row r="272" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A272">
         <f t="shared" si="5"/>
         <v>544</v>
@@ -4094,7 +4141,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="273" spans="1:3">
+    <row r="273" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A273">
         <f t="shared" si="5"/>
         <v>545</v>
@@ -4106,7 +4153,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="274" spans="1:3">
+    <row r="274" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A274">
         <f t="shared" si="5"/>
         <v>546</v>
@@ -4118,7 +4165,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="275" spans="1:3">
+    <row r="275" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A275">
         <f t="shared" si="5"/>
         <v>547</v>
@@ -4130,7 +4177,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="276" spans="1:3">
+    <row r="276" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A276">
         <f t="shared" si="5"/>
         <v>548</v>
@@ -4142,7 +4189,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="277" spans="1:3">
+    <row r="277" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A277">
         <f t="shared" si="5"/>
         <v>549</v>
@@ -4154,7 +4201,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="278" spans="1:3">
+    <row r="278" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A278">
         <f t="shared" si="5"/>
         <v>550</v>
@@ -4166,7 +4213,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="279" spans="1:3">
+    <row r="279" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A279">
         <f t="shared" si="5"/>
         <v>551</v>
@@ -4178,7 +4225,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="280" spans="1:3">
+    <row r="280" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A280">
         <f t="shared" si="5"/>
         <v>552</v>
@@ -4190,7 +4237,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="281" spans="1:3">
+    <row r="281" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A281">
         <f t="shared" si="5"/>
         <v>553</v>
@@ -4202,7 +4249,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="282" spans="1:3">
+    <row r="282" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A282">
         <f t="shared" si="5"/>
         <v>554</v>
@@ -4214,7 +4261,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="283" spans="1:3">
+    <row r="283" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A283">
         <f t="shared" si="5"/>
         <v>555</v>
@@ -4226,7 +4273,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="284" spans="1:3">
+    <row r="284" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A284">
         <f t="shared" si="5"/>
         <v>556</v>
@@ -4238,7 +4285,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="285" spans="1:3">
+    <row r="285" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A285">
         <f t="shared" si="5"/>
         <v>557</v>
@@ -4250,7 +4297,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="286" spans="1:3">
+    <row r="286" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A286">
         <f t="shared" si="5"/>
         <v>558</v>
@@ -4262,7 +4309,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="287" spans="1:3">
+    <row r="287" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A287">
         <f t="shared" si="5"/>
         <v>559</v>
@@ -4274,7 +4321,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="288" spans="1:3">
+    <row r="288" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A288">
         <f t="shared" si="5"/>
         <v>560</v>
@@ -4286,7 +4333,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="289" spans="1:3">
+    <row r="289" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A289">
         <f t="shared" si="5"/>
         <v>561</v>
@@ -4298,7 +4345,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="290" spans="1:3">
+    <row r="290" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A290">
         <f t="shared" si="5"/>
         <v>562</v>
@@ -4310,7 +4357,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="291" spans="1:3">
+    <row r="291" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A291">
         <f t="shared" si="5"/>
         <v>563</v>
@@ -4322,7 +4369,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="292" spans="1:3">
+    <row r="292" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A292">
         <f t="shared" si="5"/>
         <v>564</v>
@@ -4334,7 +4381,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="293" spans="1:3">
+    <row r="293" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A293">
         <f t="shared" si="5"/>
         <v>565</v>
@@ -4346,7 +4393,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="294" spans="1:3">
+    <row r="294" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A294">
         <v>566</v>
       </c>
@@ -4357,7 +4404,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="295" spans="1:3">
+    <row r="295" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A295">
         <v>567</v>
       </c>
@@ -4368,7 +4415,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="296" spans="1:3">
+    <row r="296" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A296">
         <v>568</v>
       </c>
@@ -4379,7 +4426,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="297" spans="1:3">
+    <row r="297" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A297">
         <v>569</v>
       </c>
@@ -4390,7 +4437,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="298" spans="1:3">
+    <row r="298" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A298">
         <v>570</v>
       </c>
@@ -4401,7 +4448,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="299" spans="1:3">
+    <row r="299" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A299">
         <v>571</v>
       </c>
@@ -4412,7 +4459,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="300" spans="1:3">
+    <row r="300" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A300">
         <v>572</v>
       </c>
@@ -4423,7 +4470,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="301" spans="1:3">
+    <row r="301" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A301">
         <v>573</v>
       </c>
@@ -4434,7 +4481,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="302" spans="1:3">
+    <row r="302" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A302">
         <v>574</v>
       </c>
@@ -4445,7 +4492,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="303" spans="1:3">
+    <row r="303" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A303">
         <v>575</v>
       </c>
@@ -4456,7 +4503,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="304" spans="1:3">
+    <row r="304" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A304">
         <v>576</v>
       </c>
@@ -4467,7 +4514,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="305" spans="1:3">
+    <row r="305" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A305">
         <v>577</v>
       </c>
@@ -4478,7 +4525,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="306" spans="1:3">
+    <row r="306" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A306">
         <v>578</v>
       </c>
@@ -4489,7 +4536,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="307" spans="1:3">
+    <row r="307" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A307">
         <v>579</v>
       </c>
@@ -4500,7 +4547,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="308" spans="1:3">
+    <row r="308" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A308">
         <v>580</v>
       </c>
@@ -4511,7 +4558,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="309" spans="1:3">
+    <row r="309" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A309">
         <v>581</v>
       </c>
@@ -4522,7 +4569,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="310" spans="1:3">
+    <row r="310" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A310">
         <v>582</v>
       </c>
@@ -4533,7 +4580,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="311" spans="1:3">
+    <row r="311" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A311">
         <v>583</v>
       </c>
@@ -4542,6 +4589,619 @@
       </c>
       <c r="C311" t="s">
         <v>134</v>
+      </c>
+    </row>
+    <row r="312" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A312">
+        <v>584</v>
+      </c>
+      <c r="B312" t="s">
+        <v>3</v>
+      </c>
+      <c r="C312" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="313" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A313">
+        <v>585</v>
+      </c>
+      <c r="B313" t="s">
+        <v>42</v>
+      </c>
+      <c r="C313" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="314" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A314">
+        <f>A313+1</f>
+        <v>586</v>
+      </c>
+      <c r="B314" t="s">
+        <v>92</v>
+      </c>
+      <c r="C314" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="315" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A315">
+        <f t="shared" ref="A315:A343" si="6">A314+1</f>
+        <v>587</v>
+      </c>
+      <c r="B315" t="s">
+        <v>93</v>
+      </c>
+      <c r="C315" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="316" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A316">
+        <f t="shared" si="6"/>
+        <v>588</v>
+      </c>
+      <c r="B316" t="s">
+        <v>51</v>
+      </c>
+      <c r="C316" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="317" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A317">
+        <f t="shared" si="6"/>
+        <v>589</v>
+      </c>
+      <c r="B317" t="s">
+        <v>3</v>
+      </c>
+      <c r="C317" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="318" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A318">
+        <f t="shared" si="6"/>
+        <v>590</v>
+      </c>
+      <c r="B318" t="s">
+        <v>135</v>
+      </c>
+      <c r="C318" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="319" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A319">
+        <f t="shared" si="6"/>
+        <v>591</v>
+      </c>
+      <c r="B319" t="s">
+        <v>61</v>
+      </c>
+      <c r="C319" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="320" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A320">
+        <f t="shared" si="6"/>
+        <v>592</v>
+      </c>
+      <c r="B320" t="s">
+        <v>61</v>
+      </c>
+      <c r="C320" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="321" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A321">
+        <f t="shared" si="6"/>
+        <v>593</v>
+      </c>
+      <c r="B321" t="s">
+        <v>66</v>
+      </c>
+      <c r="C321" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="322" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A322">
+        <f t="shared" si="6"/>
+        <v>594</v>
+      </c>
+      <c r="B322" t="s">
+        <v>21</v>
+      </c>
+      <c r="C322" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="323" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A323">
+        <f t="shared" si="6"/>
+        <v>595</v>
+      </c>
+      <c r="B323" t="s">
+        <v>79</v>
+      </c>
+      <c r="C323" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="324" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A324">
+        <f t="shared" si="6"/>
+        <v>596</v>
+      </c>
+      <c r="B324" t="s">
+        <v>30</v>
+      </c>
+      <c r="C324" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="325" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A325">
+        <f t="shared" si="6"/>
+        <v>597</v>
+      </c>
+      <c r="B325" t="s">
+        <v>98</v>
+      </c>
+      <c r="C325" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="326" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A326">
+        <f t="shared" si="6"/>
+        <v>598</v>
+      </c>
+      <c r="B326" t="s">
+        <v>97</v>
+      </c>
+      <c r="C326" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="327" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A327">
+        <f t="shared" si="6"/>
+        <v>599</v>
+      </c>
+      <c r="B327" t="s">
+        <v>78</v>
+      </c>
+      <c r="C327" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="328" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A328">
+        <f t="shared" si="6"/>
+        <v>600</v>
+      </c>
+      <c r="B328" t="s">
+        <v>7</v>
+      </c>
+      <c r="C328" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="329" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A329">
+        <f t="shared" si="6"/>
+        <v>601</v>
+      </c>
+      <c r="B329" t="s">
+        <v>88</v>
+      </c>
+      <c r="C329" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="330" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A330">
+        <f t="shared" si="6"/>
+        <v>602</v>
+      </c>
+      <c r="B330" t="s">
+        <v>39</v>
+      </c>
+      <c r="C330" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="331" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A331">
+        <f t="shared" si="6"/>
+        <v>603</v>
+      </c>
+      <c r="B331" t="s">
+        <v>65</v>
+      </c>
+      <c r="C331" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="332" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A332">
+        <f t="shared" si="6"/>
+        <v>604</v>
+      </c>
+      <c r="B332" t="s">
+        <v>30</v>
+      </c>
+      <c r="C332" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="333" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A333">
+        <f t="shared" si="6"/>
+        <v>605</v>
+      </c>
+      <c r="B333" t="s">
+        <v>34</v>
+      </c>
+      <c r="C333" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="334" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A334">
+        <f t="shared" si="6"/>
+        <v>606</v>
+      </c>
+      <c r="B334" t="s">
+        <v>59</v>
+      </c>
+      <c r="C334" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="335" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A335">
+        <f t="shared" si="6"/>
+        <v>607</v>
+      </c>
+      <c r="B335" t="s">
+        <v>47</v>
+      </c>
+      <c r="C335" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="336" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A336">
+        <f t="shared" si="6"/>
+        <v>608</v>
+      </c>
+      <c r="B336" t="s">
+        <v>87</v>
+      </c>
+      <c r="C336" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="337" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A337">
+        <f t="shared" si="6"/>
+        <v>609</v>
+      </c>
+      <c r="B337" t="s">
+        <v>137</v>
+      </c>
+      <c r="C337" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="338" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A338">
+        <f t="shared" si="6"/>
+        <v>610</v>
+      </c>
+      <c r="B338" t="s">
+        <v>17</v>
+      </c>
+      <c r="C338" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="339" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A339">
+        <f t="shared" si="6"/>
+        <v>611</v>
+      </c>
+      <c r="B339" t="s">
+        <v>55</v>
+      </c>
+      <c r="C339" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="340" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A340">
+        <f t="shared" si="6"/>
+        <v>612</v>
+      </c>
+      <c r="B340" t="s">
+        <v>78</v>
+      </c>
+      <c r="C340" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="341" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A341">
+        <f t="shared" si="6"/>
+        <v>613</v>
+      </c>
+      <c r="B341" t="s">
+        <v>0</v>
+      </c>
+      <c r="C341" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="342" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A342">
+        <f t="shared" si="6"/>
+        <v>614</v>
+      </c>
+      <c r="B342" t="s">
+        <v>138</v>
+      </c>
+      <c r="C342" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="343" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A343">
+        <f t="shared" si="6"/>
+        <v>615</v>
+      </c>
+      <c r="B343" t="s">
+        <v>25</v>
+      </c>
+      <c r="C343" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="344" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A344">
+        <v>616</v>
+      </c>
+      <c r="B344" t="s">
+        <v>22</v>
+      </c>
+      <c r="C344" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="345" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A345">
+        <v>617</v>
+      </c>
+      <c r="B345" t="s">
+        <v>105</v>
+      </c>
+      <c r="C345" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="346" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A346">
+        <v>618</v>
+      </c>
+      <c r="B346" t="s">
+        <v>3</v>
+      </c>
+      <c r="C346" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="347" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A347">
+        <v>619</v>
+      </c>
+      <c r="B347" t="s">
+        <v>104</v>
+      </c>
+      <c r="C347" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="348" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A348">
+        <v>620</v>
+      </c>
+      <c r="B348" t="s">
+        <v>61</v>
+      </c>
+      <c r="C348" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="349" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A349">
+        <v>621</v>
+      </c>
+      <c r="B349" t="s">
+        <v>43</v>
+      </c>
+      <c r="C349" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="350" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A350">
+        <v>622</v>
+      </c>
+      <c r="B350" t="s">
+        <v>34</v>
+      </c>
+      <c r="C350" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="351" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A351">
+        <v>623</v>
+      </c>
+      <c r="B351" t="s">
+        <v>73</v>
+      </c>
+      <c r="C351" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="352" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A352">
+        <v>624</v>
+      </c>
+      <c r="B352" t="s">
+        <v>42</v>
+      </c>
+      <c r="C352" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="353" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A353">
+        <v>2183</v>
+      </c>
+      <c r="B353" t="s">
+        <v>22</v>
+      </c>
+      <c r="C353" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="354" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A354">
+        <v>2184</v>
+      </c>
+      <c r="B354" t="s">
+        <v>22</v>
+      </c>
+      <c r="C354" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="355" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A355">
+        <v>2185</v>
+      </c>
+      <c r="B355" t="s">
+        <v>61</v>
+      </c>
+      <c r="C355" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="356" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A356">
+        <v>2186</v>
+      </c>
+      <c r="B356" t="s">
+        <v>66</v>
+      </c>
+      <c r="C356" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="357" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A357">
+        <v>2187</v>
+      </c>
+      <c r="B357" t="s">
+        <v>140</v>
+      </c>
+      <c r="C357" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="358" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A358">
+        <v>2188</v>
+      </c>
+      <c r="B358" t="s">
+        <v>105</v>
+      </c>
+      <c r="C358" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="359" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A359">
+        <v>2189</v>
+      </c>
+      <c r="B359" t="s">
+        <v>78</v>
+      </c>
+      <c r="C359" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="360" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A360">
+        <v>2190</v>
+      </c>
+      <c r="B360" t="s">
+        <v>30</v>
+      </c>
+      <c r="C360" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="361" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A361">
+        <v>2191</v>
+      </c>
+      <c r="B361" t="s">
+        <v>65</v>
+      </c>
+      <c r="C361" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="362" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A362">
+        <v>2192</v>
+      </c>
+      <c r="B362" t="s">
+        <v>34</v>
+      </c>
+      <c r="C362" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="363" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A363">
+        <v>2193</v>
+      </c>
+      <c r="B363" t="s">
+        <v>108</v>
+      </c>
+      <c r="C363" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="364" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A364">
+        <v>2194</v>
+      </c>
+      <c r="B364" t="s">
+        <v>10</v>
+      </c>
+      <c r="C364" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>